<commit_message>
el KCC0 ya no sale
</commit_message>
<xml_diff>
--- a/Data_TicketPromedio.xlsx
+++ b/Data_TicketPromedio.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="33">
   <si>
     <t>Distribuidora</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>(KCC2) Mesa 2</t>
-  </si>
-  <si>
-    <t>(KCC0) Oficina</t>
   </si>
 </sst>
 </file>
@@ -462,7 +459,7 @@
   <dimension ref="B3:G158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3309,7 +3306,7 @@
         <v>40.700000000000003</v>
       </c>
       <c r="G144">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145" spans="2:7" x14ac:dyDescent="0.25">
@@ -3329,7 +3326,7 @@
         <v>8499.5400000000009</v>
       </c>
       <c r="G145">
-        <v>0</v>
+        <v>153</v>
       </c>
     </row>
     <row r="146" spans="2:7" x14ac:dyDescent="0.25">
@@ -3349,7 +3346,7 @@
         <v>2234.41</v>
       </c>
       <c r="G146">
-        <v>0</v>
+        <v>57</v>
       </c>
     </row>
     <row r="147" spans="2:7" x14ac:dyDescent="0.25">
@@ -3369,7 +3366,7 @@
         <v>535.66999999999996</v>
       </c>
       <c r="G147">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="148" spans="2:7" x14ac:dyDescent="0.25">
@@ -3389,7 +3386,7 @@
         <v>87329.62</v>
       </c>
       <c r="G148">
-        <v>0</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="149" spans="2:7" x14ac:dyDescent="0.25">
@@ -3409,7 +3406,7 @@
         <v>77969.83</v>
       </c>
       <c r="G149">
-        <v>0</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="150" spans="2:7" x14ac:dyDescent="0.25">
@@ -3429,7 +3426,7 @@
         <v>182.67</v>
       </c>
       <c r="G150">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="151" spans="2:7" x14ac:dyDescent="0.25">
@@ -3449,7 +3446,7 @@
         <v>20567.54</v>
       </c>
       <c r="G151">
-        <v>0</v>
+        <v>643</v>
       </c>
     </row>
     <row r="152" spans="2:7" x14ac:dyDescent="0.25">
@@ -3469,7 +3466,7 @@
         <v>9699.6</v>
       </c>
       <c r="G152">
-        <v>0</v>
+        <v>294</v>
       </c>
     </row>
     <row r="153" spans="2:7" x14ac:dyDescent="0.25">
@@ -3483,13 +3480,13 @@
         <v>10</v>
       </c>
       <c r="E153" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F153">
         <v>1112.2</v>
       </c>
       <c r="G153">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="154" spans="2:7" x14ac:dyDescent="0.25">
@@ -3509,7 +3506,7 @@
         <v>174046.29</v>
       </c>
       <c r="G154">
-        <v>0</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="155" spans="2:7" x14ac:dyDescent="0.25">
@@ -3529,7 +3526,7 @@
         <v>122175.01</v>
       </c>
       <c r="G155">
-        <v>0</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="156" spans="2:7" x14ac:dyDescent="0.25">
@@ -3549,7 +3546,7 @@
         <v>353.16</v>
       </c>
       <c r="G156">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="157" spans="2:7" x14ac:dyDescent="0.25">
@@ -3569,7 +3566,7 @@
         <v>57649.59</v>
       </c>
       <c r="G157">
-        <v>0</v>
+        <v>665</v>
       </c>
     </row>
     <row r="158" spans="2:7" x14ac:dyDescent="0.25">
@@ -3589,7 +3586,7 @@
         <v>32271.17</v>
       </c>
       <c r="G158">
-        <v>0</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>